<commit_message>
added parts list and orders
</commit_message>
<xml_diff>
--- a/BOMs&Parts List/Cameron Parts on Hand.xlsx
+++ b/BOMs&Parts List/Cameron Parts on Hand.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6700" yWindow="21600" windowWidth="12800" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -587,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -617,13 +617,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -631,7 +628,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -639,61 +636,64 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
         <v>5</v>
       </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -701,80 +701,89 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
         <v>5</v>
       </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -782,7 +791,7 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -795,119 +804,110 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>36</v>
+      <c r="A28">
+        <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>2</v>
-      </c>
-      <c r="B31" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>2</v>
-      </c>
-      <c r="B32" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
-        <v>4</v>
-      </c>
-      <c r="B34" t="s">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35">
-        <v>4</v>
-      </c>
-      <c r="B35" t="s">
-        <v>48</v>
+      <c r="A35" t="s">
+        <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -946,11 +946,13 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A4:C35">
+    <sortCondition ref="C35"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>